<commit_message>
Advancing on process_input_data() func
</commit_message>
<xml_diff>
--- a/model_features.xlsx
+++ b/model_features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paulo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738E9987-010D-4C83-833A-19D10EB99DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33409D5-C390-49EA-9B3D-3F981FDFB24A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CEA1B408-EAEC-43DA-A9D5-654FAEA6FD4C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="50">
   <si>
     <t>bedrooms</t>
   </si>
@@ -178,16 +178,30 @@
   </si>
   <si>
     <t>zipcode_demographics.csv</t>
+  </si>
+  <si>
+    <t>Key Value</t>
+  </si>
+  <si>
+    <t>Model Features</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -201,18 +215,66 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -221,10 +283,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,18 +612,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAA31EDD-0983-4E4A-835F-E2B7C709C479}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
@@ -579,315 +654,327 @@
     <col min="33" max="33" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="F1" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D2" s="1"/>
+      <c r="F2" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="F3" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="F4" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="10" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="9" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="9" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="9" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Restructuring config files and creating dynamic input schema for Sales Data (bonus endpoint)
</commit_message>
<xml_diff>
--- a/model_features.xlsx
+++ b/model_features.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paulo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paulo\Documents\repos\mle-project-challenge-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33409D5-C390-49EA-9B3D-3F981FDFB24A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3F4465-81A2-4B6F-A464-A4BD2DADC38E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CEA1B408-EAEC-43DA-A9D5-654FAEA6FD4C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CEA1B408-EAEC-43DA-A9D5-654FAEA6FD4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="71">
   <si>
     <t>bedrooms</t>
   </si>
@@ -184,6 +185,69 @@
   </si>
   <si>
     <t>Model Features</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>bathrooms</t>
+  </si>
+  <si>
+    <t>sqft_living</t>
+  </si>
+  <si>
+    <t>sqft_lot</t>
+  </si>
+  <si>
+    <t>floors</t>
+  </si>
+  <si>
+    <t>waterfront</t>
+  </si>
+  <si>
+    <t>view</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>grade</t>
+  </si>
+  <si>
+    <t>sqft_above</t>
+  </si>
+  <si>
+    <t>sqft_basement</t>
+  </si>
+  <si>
+    <t>yr_built</t>
+  </si>
+  <si>
+    <t>yr_renovated</t>
+  </si>
+  <si>
+    <t>zipcode</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>sqft_living15</t>
+  </si>
+  <si>
+    <t>sqft_lot15</t>
+  </si>
+  <si>
+    <t>kc_house_data.csv</t>
   </si>
 </sst>
 </file>
@@ -215,7 +279,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -243,6 +307,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -283,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -298,6 +368,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAA31EDD-0983-4E4A-835F-E2B7C709C479}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,4 +1055,345 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CAEF35A-E392-4CC7-987A-74D113B33805}">
+  <dimension ref="A1:C34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>